<commit_message>
Update SUSPENDER (version 1).xlsb.xlsx
</commit_message>
<xml_diff>
--- a/SUSPENDER (version 1).xlsb.xlsx
+++ b/SUSPENDER (version 1).xlsb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Servicio al Cliente\Downloads\Mora\Mora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5ADAA6D-5F48-4A36-8B8C-313FF32A6ADE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757DEC0B-0927-4340-A2AA-661ADCA4D635}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{96D49413-507F-423F-95B6-C78EBA344D61}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1866" uniqueCount="819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1867" uniqueCount="819">
   <si>
     <t>N° Abonado</t>
   </si>
@@ -2915,7 +2915,7 @@
   <dimension ref="A1:N362"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="H68" sqref="H68"/>
+      <selection activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5889,45 +5889,47 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A69" s="4">
+    <row r="69" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="8">
         <v>1917</v>
       </c>
-      <c r="B69" s="4">
+      <c r="B69" s="8">
         <v>15924755</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="C69" s="8" t="s">
         <v>560</v>
       </c>
-      <c r="D69" s="4">
+      <c r="D69" s="8">
         <v>57000</v>
       </c>
-      <c r="E69" s="4">
+      <c r="E69" s="8">
         <v>57000</v>
       </c>
-      <c r="F69" s="13">
+      <c r="F69" s="14">
         <v>3126656075</v>
       </c>
-      <c r="G69" s="5"/>
-      <c r="H69" t="s">
-        <v>20</v>
-      </c>
-      <c r="I69" t="s">
+      <c r="G69" s="9" t="s">
+        <v>814</v>
+      </c>
+      <c r="H69" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I69" s="10" t="s">
         <v>537</v>
       </c>
-      <c r="J69" t="s">
+      <c r="J69" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K69" t="s">
+      <c r="K69" s="10" t="s">
         <v>513</v>
       </c>
-      <c r="L69" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M69" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N69" s="6" t="e">
+      <c r="L69" s="10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M69" s="10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N69" s="11" t="e">
         <v>#N/A</v>
       </c>
     </row>

</xml_diff>